<commit_message>
Asignación de Recursos y Nuevos datos para economiua
</commit_message>
<xml_diff>
--- a/Factibilidad Economica - Cálculos LoRa con Bat 7Ah.xlsx
+++ b/Factibilidad Economica - Cálculos LoRa con Bat 7Ah.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis Quiroga\Desktop\Facu\Proyecto\Software\Planillas de materiales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis Quiroga\Desktop\Facu\Industrias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC12B8C9-92FB-459B-8D32-303E48D4255F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46AD85-6923-44A4-9E74-E62EC124E22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Costos indirectos</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Inversion inicial total USD</t>
   </si>
   <si>
-    <t>Costo del producto con criterio de geloso</t>
-  </si>
-  <si>
     <t>No voy a invertir todo de una, sino de a poco pero llegando a ese monto</t>
   </si>
   <si>
@@ -140,6 +137,24 @@
   <si>
     <t>La primera tanda en 18 meses será el equivalente de 70 unidades.</t>
   </si>
+  <si>
+    <t>Costo del producto con criterio de ecuacion</t>
+  </si>
+  <si>
+    <t>Salario en Dolares</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Técnico de Ensamblado(1)</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,6 +234,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -240,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -263,11 +285,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +373,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -332,6 +392,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,8 +619,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -566,13 +632,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.2">
-      <c r="A1" s="21" t="s">
-        <v>35</v>
+      <c r="A1" s="25" t="s">
+        <v>34</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -958,7 +1024,7 @@
     </row>
     <row r="12" spans="1:26" ht="13.2">
       <c r="A12" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="16">
         <f>B11/70</f>
@@ -1089,7 +1155,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="15">
         <f>G10*10</f>
@@ -1129,7 +1195,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1162,7 +1228,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="27" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="1"/>
@@ -1192,7 +1258,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="13"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="23"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1219,10 +1285,10 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="17" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="23"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1253,7 +1319,7 @@
         <v>2831.5359584633857</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1280,10 +1346,10 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="23"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1306,17 +1372,17 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="13.2">
-      <c r="A23" s="24" t="s">
-        <v>31</v>
+      <c r="A23" s="28" t="s">
+        <v>30</v>
       </c>
-      <c r="B23" s="24"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="1"/>
       <c r="D23" s="18">
         <f>B18*(1-0.35-0.03)/(1-0.35-0.03-0.47)</f>
         <v>3209.074086258503</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="23"/>
+      <c r="F23" s="27"/>
       <c r="G23" s="15">
         <f>B10*6</f>
         <v>10476.190476190477</v>
@@ -1346,7 +1412,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1413,7 +1479,7 @@
       <c r="C26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1464,9 +1530,18 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1491,9 +1566,21 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="13.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="22">
+        <f>(70000*1.17*1.23)/105</f>
+        <v>959.4</v>
+      </c>
+      <c r="C29" s="23">
+        <f>B29/20</f>
+        <v>47.97</v>
+      </c>
+      <c r="D29" s="24">
+        <f>C29/8</f>
+        <v>5.9962499999999999</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1518,9 +1605,21 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="13.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="A30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="22">
+        <f xml:space="preserve"> (80000*1.17*1.23)/105</f>
+        <v>1096.4571428571428</v>
+      </c>
+      <c r="C30" s="23">
+        <f t="shared" ref="C30:C32" si="0">B30/20</f>
+        <v>54.822857142857139</v>
+      </c>
+      <c r="D30" s="24">
+        <f t="shared" ref="D30:D32" si="1">C30/8</f>
+        <v>6.8528571428571423</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1545,10 +1644,21 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="13.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="22">
+        <f xml:space="preserve"> (120000*1.17*1.23)/105</f>
+        <v>1644.6857142857143</v>
+      </c>
+      <c r="C31" s="23">
+        <f t="shared" si="0"/>
+        <v>82.234285714285718</v>
+      </c>
+      <c r="D31" s="24">
+        <f t="shared" si="1"/>
+        <v>10.279285714285715</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1573,10 +1683,21 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="13.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="A32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="22">
+        <f xml:space="preserve"> (85000*1.17*1.23)/(105)</f>
+        <v>1164.9857142857143</v>
+      </c>
+      <c r="C32" s="23">
+        <f t="shared" si="0"/>
+        <v>58.249285714285712</v>
+      </c>
+      <c r="D32" s="24">
+        <f t="shared" si="1"/>
+        <v>7.281160714285714</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1601,10 +1722,14 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="13.2">
-      <c r="A33" s="1"/>
+      <c r="A33" s="29" t="s">
+        <v>40</v>
+      </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="30">
+        <v>8</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -28711,6 +28836,6 @@
     <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nueva Asignación de recursos antes de reunión con tutor
</commit_message>
<xml_diff>
--- a/Factibilidad Economica - Cálculos LoRa con Bat 7Ah.xlsx
+++ b/Factibilidad Economica - Cálculos LoRa con Bat 7Ah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis Quiroga\Desktop\Facu\Industrias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46AD85-6923-44A4-9E74-E62EC124E22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4002605-0D02-43D0-895C-04C3B7DB3787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Costos indirectos</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Costo Total (ARS)</t>
-  </si>
-  <si>
-    <t>Electricidad + Agua + Gas</t>
   </si>
   <si>
     <t>TOTAL 1 MES</t>
@@ -102,9 +99,6 @@
     <t>Equipo de Ingeniería/ Jefe de Proyecto (1)</t>
   </si>
   <si>
-    <t>Limpieza</t>
-  </si>
-  <si>
     <t>Inversión  inicial</t>
   </si>
   <si>
@@ -155,6 +149,60 @@
   <si>
     <t>Técnico de Ensamblado(1)</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Costo MOD</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Damian</t>
+  </si>
+  <si>
+    <t>Adrián</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Costos por Tarea</t>
+  </si>
+  <si>
+    <t>Investigacion</t>
+  </si>
+  <si>
+    <t>Planificacion</t>
+  </si>
+  <si>
+    <t>Ingeniería</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Programación</t>
+  </si>
+  <si>
+    <t>Construcción</t>
+  </si>
+  <si>
+    <t>Ensayos</t>
+  </si>
+  <si>
+    <t>Pruebas de funcionamiento</t>
+  </si>
+  <si>
+    <t>Testing Final</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
 </sst>
 </file>
 
@@ -163,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,6 +289,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -262,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -313,11 +368,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,9 +502,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,6 +509,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,11 +548,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,8 +771,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -632,13 +784,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.2">
-      <c r="A1" s="25" t="s">
-        <v>34</v>
+      <c r="A1" s="35" t="s">
+        <v>32</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -723,7 +875,7 @@
     </row>
     <row r="4" spans="1:26" ht="13.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5">
         <f>70000/(105*3)</f>
@@ -737,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>4</v>
@@ -763,7 +915,7 @@
     </row>
     <row r="5" spans="1:26" ht="13.2">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5">
         <f xml:space="preserve"> 80000/(105*3)</f>
@@ -771,7 +923,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
@@ -805,7 +957,7 @@
     </row>
     <row r="6" spans="1:26" ht="13.2">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5">
         <f xml:space="preserve"> 120000/(105*2)</f>
@@ -813,17 +965,17 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
       <c r="F6" s="9">
-        <v>180.26929999999999</v>
+        <v>181.28569999999999</v>
       </c>
       <c r="G6" s="9">
         <f>F6*E6</f>
-        <v>180.26929999999999</v>
+        <v>181.28569999999999</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -847,7 +999,7 @@
     </row>
     <row r="7" spans="1:26" ht="13.2">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5">
         <f xml:space="preserve"> 90000/(105*2)</f>
@@ -855,7 +1007,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="9">
         <v>1</v>
@@ -887,13 +1039,8 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.2">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="5">
-        <f>55000/(105*3)</f>
-        <v>174.60317460317461</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
@@ -920,13 +1067,8 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.2">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5">
-        <f>10000/105</f>
-        <v>95.238095238095241</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
@@ -954,21 +1096,21 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="10">
         <f>SUM(B4:B9)</f>
-        <v>1746.031746031746</v>
+        <v>1476.1904761904761</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="16">
         <f>SUM(G5:G9)</f>
-        <v>327.40929999999997</v>
+        <v>328.42570000000001</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -992,11 +1134,11 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="10">
         <f>18*B10</f>
-        <v>31428.571428571428</v>
+        <v>26571.428571428572</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
@@ -1024,11 +1166,11 @@
     </row>
     <row r="12" spans="1:26" ht="13.2">
       <c r="A12" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="16">
         <f>B11/70</f>
-        <v>448.9795918367347</v>
+        <v>379.59183673469391</v>
       </c>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
@@ -1083,7 +1225,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1118,7 +1260,7 @@
       <c r="D15" s="13"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1143,23 +1285,23 @@
     </row>
     <row r="16" spans="1:26" ht="13.2">
       <c r="A16" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="12">
         <f>G10</f>
-        <v>327.40929999999997</v>
+        <v>328.42570000000001</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="15">
         <f>G10*10</f>
-        <v>3274.0929999999998</v>
+        <v>3284.2570000000001</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1183,19 +1325,19 @@
     </row>
     <row r="17" spans="1:26" ht="13.2">
       <c r="A17" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="12">
         <f>B12</f>
-        <v>448.9795918367347</v>
+        <v>379.59183673469391</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1220,16 +1362,16 @@
     </row>
     <row r="18" spans="1:26" ht="13.2" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="16">
         <f>SUM(B16:B17)</f>
-        <v>776.38889183673473</v>
+        <v>708.01753673469398</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="27" t="s">
-        <v>25</v>
+      <c r="F18" s="37" t="s">
+        <v>23</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1258,7 +1400,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="13"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1285,10 +1427,10 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1316,10 +1458,10 @@
       <c r="C21" s="1"/>
       <c r="D21" s="18">
         <f>B18*(1-0.35-0.03)/(1-0.35-0.03-0.45)</f>
-        <v>2831.5359584633857</v>
+        <v>2582.1816045618252</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1346,10 +1488,10 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="27"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1372,20 +1514,20 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="13.2">
-      <c r="A23" s="28" t="s">
-        <v>30</v>
+      <c r="A23" s="38" t="s">
+        <v>28</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="1"/>
       <c r="D23" s="18">
         <f>B18*(1-0.35-0.03)/(1-0.35-0.03-0.47)</f>
-        <v>3209.074086258503</v>
+        <v>2926.472485170068</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="27"/>
+      <c r="F23" s="37"/>
       <c r="G23" s="15">
         <f>B10*6</f>
-        <v>10476.190476190477</v>
+        <v>8857.1428571428569</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1412,7 +1554,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1443,15 +1585,15 @@
       <c r="C25" s="1"/>
       <c r="D25" s="18">
         <f>B18*(1-0.35-0.03)/(1-0.35-0.03-0.49)</f>
-        <v>3702.7777918367347</v>
+        <v>3376.699021350079</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G25" s="15">
         <f>G23+G16</f>
-        <v>13750.283476190478</v>
+        <v>12141.399857142856</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1479,7 +1621,7 @@
       <c r="C26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1530,17 +1672,17 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" s="34" t="s">
         <v>37</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>39</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1566,18 +1708,18 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="13.2">
-      <c r="A29" s="4" t="s">
-        <v>13</v>
+      <c r="A29" s="30" t="s">
+        <v>12</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="31">
         <f>(70000*1.17*1.23)/105</f>
         <v>959.4</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="32">
         <f>B29/20</f>
         <v>47.97</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="33">
         <f>C29/8</f>
         <v>5.9962499999999999</v>
       </c>
@@ -1606,17 +1748,17 @@
     </row>
     <row r="30" spans="1:26" ht="13.2">
       <c r="A30" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="21">
         <f xml:space="preserve"> (80000*1.17*1.23)/105</f>
         <v>1096.4571428571428</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <f t="shared" ref="C30:C32" si="0">B30/20</f>
         <v>54.822857142857139</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <f t="shared" ref="D30:D32" si="1">C30/8</f>
         <v>6.8528571428571423</v>
       </c>
@@ -1645,17 +1787,17 @@
     </row>
     <row r="31" spans="1:26" ht="13.2">
       <c r="A31" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="21">
         <f xml:space="preserve"> (120000*1.17*1.23)/105</f>
         <v>1644.6857142857143</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="22">
         <f t="shared" si="0"/>
         <v>82.234285714285718</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="23">
         <f t="shared" si="1"/>
         <v>10.279285714285715</v>
       </c>
@@ -1683,18 +1825,18 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="13.2">
-      <c r="A32" s="4" t="s">
-        <v>20</v>
+      <c r="A32" s="24" t="s">
+        <v>19</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="25">
         <f xml:space="preserve"> (85000*1.17*1.23)/(105)</f>
         <v>1164.9857142857143</v>
       </c>
-      <c r="C32" s="23">
+      <c r="C32" s="26">
         <f t="shared" si="0"/>
         <v>58.249285714285712</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="27">
         <f t="shared" si="1"/>
         <v>7.281160714285714</v>
       </c>
@@ -1722,13 +1864,17 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="13.2">
-      <c r="A33" s="29" t="s">
-        <v>40</v>
+      <c r="A33" s="28" t="s">
+        <v>38</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="30">
-        <v>8</v>
+      <c r="B33" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="29">
+        <v>10</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1810,8 +1956,10 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="13.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="22"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1838,8 +1986,12 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="13.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="22">
+        <v>11589.76</v>
+      </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1866,8 +2018,12 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="13.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="A38" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="22">
+        <v>10352.16</v>
+      </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1894,8 +2050,12 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="13.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="A39" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="22">
+        <v>1200.1199999999999</v>
+      </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1922,8 +2082,12 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="13.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="A40" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="22">
+        <v>1576.57</v>
+      </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1950,8 +2114,12 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="13.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="A41" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="22">
+        <v>1040</v>
+      </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2034,8 +2202,10 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="13.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="22"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2062,8 +2232,12 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="13.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="A45" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="22">
+        <v>6955.5</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2090,8 +2264,12 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="13.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="A46" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="22">
+        <v>2414</v>
+      </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2118,8 +2296,12 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="13.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="A47" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="22">
+        <v>6281.08</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2146,8 +2328,12 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="13.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="22">
+        <v>2820.29</v>
+      </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2174,8 +2360,12 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="13.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="A49" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="22">
+        <v>2879.5</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2202,8 +2392,12 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="13.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="A50" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="22">
+        <v>447.52</v>
+      </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2230,8 +2424,12 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="13.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+      <c r="A51" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="22">
+        <v>212.12</v>
+      </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2258,8 +2456,12 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="13.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="A52" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="22">
+        <v>1427.4</v>
+      </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2286,8 +2488,12 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="13.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="A53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="22">
+        <v>993.2</v>
+      </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2314,8 +2520,12 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="13.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="22">
+        <v>1328</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2342,8 +2552,11 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="13.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="34">
+        <f>SUM(B45:B54)</f>
+        <v>25758.61</v>
+      </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>

</xml_diff>